<commit_message>
working on testing shot distances, speeds
</commit_message>
<xml_diff>
--- a/Power Cell Ballistics.xlsx
+++ b/Power Cell Ballistics.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timfu\Documents\2020 FRC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\Code\FRC\2020-Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D14CA52-EB12-4353-B9C4-4433DCB78A82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BECA7C2-ABCB-4478-9835-84FB0737CB9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="1" activeTab="1" xr2:uid="{6505FE35-6DDB-4B85-B29F-6D89AE1E982C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="1" xr2:uid="{6505FE35-6DDB-4B85-B29F-6D89AE1E982C}"/>
   </bookViews>
   <sheets>
     <sheet name="Height" sheetId="2" r:id="rId1"/>
     <sheet name="Ballistics" sheetId="7" r:id="rId2"/>
-    <sheet name="Distance" sheetId="3" r:id="rId3"/>
-    <sheet name="Defense" sheetId="8" r:id="rId4"/>
-    <sheet name="Locations" sheetId="9" r:id="rId5"/>
-    <sheet name="Plot Data" sheetId="1" r:id="rId6"/>
-    <sheet name="Motor Speed Estimator" sheetId="6" r:id="rId7"/>
+    <sheet name="DistanceSpeedTesting" sheetId="10" r:id="rId3"/>
+    <sheet name="Distance" sheetId="3" r:id="rId4"/>
+    <sheet name="Defense" sheetId="8" r:id="rId5"/>
+    <sheet name="Locations" sheetId="9" r:id="rId6"/>
+    <sheet name="Plot Data" sheetId="1" r:id="rId7"/>
+    <sheet name="Motor Speed Estimator" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="69">
   <si>
     <t>2020 FRC - Infinite Recharge</t>
   </si>
@@ -220,6 +223,30 @@
   </si>
   <si>
     <t>Front of Trench</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Fixed 45 degree angle</t>
+  </si>
+  <si>
+    <t>all shots made</t>
+  </si>
+  <si>
+    <t>center of trench, behind wheel</t>
+  </si>
+  <si>
+    <t>immediately in front of wheel</t>
+  </si>
+  <si>
+    <t>not enough</t>
+  </si>
+  <si>
+    <t>missed 3 shots</t>
+  </si>
+  <si>
+    <t>missed 2 shots</t>
   </si>
 </sst>
 </file>
@@ -1523,109 +1550,109 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.384714431314478</c:v>
+                  <c:v>27.336596905207195</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92.769428862628956</c:v>
+                  <c:v>54.673193810414389</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>139.15414329394341</c:v>
+                  <c:v>82.009790715621577</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>185.53885772525791</c:v>
+                  <c:v>109.34638762082878</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>231.92357215657236</c:v>
+                  <c:v>136.68298452603597</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>278.30828658788681</c:v>
+                  <c:v>164.01958143124315</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>324.69300101920129</c:v>
+                  <c:v>191.35617833645034</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>371.07771545051583</c:v>
+                  <c:v>218.69277524165756</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>417.46242988183025</c:v>
+                  <c:v>246.02937214686474</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>463.84714431314472</c:v>
+                  <c:v>273.36596905207193</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>510.23185874445926</c:v>
+                  <c:v>300.70256595727915</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>556.61657317577362</c:v>
+                  <c:v>328.03916286248631</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>603.00128760708822</c:v>
+                  <c:v>355.37575976769352</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>649.38600203840258</c:v>
+                  <c:v>382.71235667290068</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>695.77071646971706</c:v>
+                  <c:v>410.0489535781079</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>742.15543090103165</c:v>
+                  <c:v>437.38555048331511</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>788.54014533234601</c:v>
+                  <c:v>464.72214738852227</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>834.92485976366049</c:v>
+                  <c:v>492.05874429372949</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>881.30957419497497</c:v>
+                  <c:v>519.39534119893665</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>927.69428862628945</c:v>
+                  <c:v>546.73193810414386</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>974.07900305760393</c:v>
+                  <c:v>574.06853500935108</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1020.4637174889185</c:v>
+                  <c:v>601.4051319145583</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1066.8484319202328</c:v>
+                  <c:v>628.7417288197654</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1113.2331463515472</c:v>
+                  <c:v>656.07832572497261</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1159.6178607828617</c:v>
+                  <c:v>683.41492263017983</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1206.0025752141764</c:v>
+                  <c:v>710.75151953538705</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1252.3872896454909</c:v>
+                  <c:v>738.08811644059426</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1298.7720040768052</c:v>
+                  <c:v>765.42471334580136</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1345.1567185081196</c:v>
+                  <c:v>792.76131025100858</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1391.5414329394341</c:v>
+                  <c:v>820.0979071562158</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1437.9261473707486</c:v>
+                  <c:v>847.43450406142301</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1484.3108618020633</c:v>
+                  <c:v>874.77110096663023</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1530.6955762333776</c:v>
+                  <c:v>902.10769787183733</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1577.080290664692</c:v>
+                  <c:v>929.44429477704455</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1623.4650050960065</c:v>
+                  <c:v>956.78089168225176</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1640,109 +1667,109 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.2471019465717816</c:v>
+                  <c:v>25.398297539033234</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.633803893143563</c:v>
+                  <c:v>46.936195078066461</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1601058397153459</c:v>
+                  <c:v>64.613692617099701</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8260077862871213</c:v>
+                  <c:v>78.430790156132929</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-7.368490267141091</c:v>
+                  <c:v>88.387487695166158</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-20.423388320569309</c:v>
+                  <c:v>94.483785234199388</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-37.338686373997518</c:v>
+                  <c:v>96.719682773232606</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-58.114384427425776</c:v>
+                  <c:v>95.095180312265825</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-82.750482480853961</c:v>
+                  <c:v>89.61027785129906</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-111.24698053428219</c:v>
+                  <c:v>80.264975390332296</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-143.60387858771043</c:v>
+                  <c:v>67.059272929365534</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-179.82117664113861</c:v>
+                  <c:v>49.993170468398773</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-219.89887469456687</c:v>
+                  <c:v>29.066668007431929</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-263.83697274799499</c:v>
+                  <c:v>4.279765546465228</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-311.63547080142325</c:v>
+                  <c:v>-24.367536914501557</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-363.29436885485165</c:v>
+                  <c:v>-56.875239375468425</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-418.81366690827963</c:v>
+                  <c:v>-93.243341836434979</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-478.19336496170797</c:v>
+                  <c:v>-133.4718442974019</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-541.43346301513611</c:v>
+                  <c:v>-177.56074675836862</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-608.53396106856439</c:v>
+                  <c:v>-225.51004921933543</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-679.49485912199259</c:v>
+                  <c:v>-277.31975168030215</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-754.31615717542093</c:v>
+                  <c:v>-332.98985414126901</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-832.99785522884883</c:v>
+                  <c:v>-392.52035660223555</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-915.53995328227722</c:v>
+                  <c:v>-455.91125906320246</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-1001.9424513357054</c:v>
+                  <c:v>-523.16256152416918</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-1092.205349389134</c:v>
+                  <c:v>-594.27426398513626</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-1186.3286474425622</c:v>
+                  <c:v>-669.24636644610302</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-1284.31234549599</c:v>
+                  <c:v>-748.07886890706948</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-1386.1564435494186</c:v>
+                  <c:v>-830.77177136803653</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-1491.8609416028467</c:v>
+                  <c:v>-917.32507382900314</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-1601.4258396562752</c:v>
+                  <c:v>-1007.7387762899702</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-1714.8511377097036</c:v>
+                  <c:v>-1102.012878750937</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-1832.1368357631311</c:v>
+                  <c:v>-1200.1473812119034</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-1953.2829338165591</c:v>
+                  <c:v>-1302.1422836728698</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-2078.2894318699882</c:v>
+                  <c:v>-1407.9975861338373</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1780,109 +1807,109 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.384714431314478</c:v>
+                  <c:v>27.336596905207195</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92.769428862628956</c:v>
+                  <c:v>54.673193810414389</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>139.15414329394341</c:v>
+                  <c:v>82.009790715621577</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>185.53885772525791</c:v>
+                  <c:v>109.34638762082878</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>231.92357215657236</c:v>
+                  <c:v>136.68298452603597</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>278.30828658788681</c:v>
+                  <c:v>164.01958143124315</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>324.69300101920129</c:v>
+                  <c:v>191.35617833645034</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>371.07771545051583</c:v>
+                  <c:v>218.69277524165756</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>417.46242988183025</c:v>
+                  <c:v>246.02937214686474</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>463.84714431314472</c:v>
+                  <c:v>273.36596905207193</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>510.23185874445926</c:v>
+                  <c:v>300.70256595727915</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>556.61657317577362</c:v>
+                  <c:v>328.03916286248631</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>603.00128760708822</c:v>
+                  <c:v>355.37575976769352</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>649.38600203840258</c:v>
+                  <c:v>382.71235667290068</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>695.77071646971706</c:v>
+                  <c:v>410.0489535781079</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>742.15543090103165</c:v>
+                  <c:v>437.38555048331511</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>788.54014533234601</c:v>
+                  <c:v>464.72214738852227</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>834.92485976366049</c:v>
+                  <c:v>492.05874429372949</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>881.30957419497497</c:v>
+                  <c:v>519.39534119893665</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>927.69428862628945</c:v>
+                  <c:v>546.73193810414386</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>974.07900305760393</c:v>
+                  <c:v>574.06853500935108</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1020.4637174889185</c:v>
+                  <c:v>601.4051319145583</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1066.8484319202328</c:v>
+                  <c:v>628.7417288197654</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1113.2331463515472</c:v>
+                  <c:v>656.07832572497261</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1159.6178607828617</c:v>
+                  <c:v>683.41492263017983</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1206.0025752141764</c:v>
+                  <c:v>710.75151953538705</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1252.3872896454909</c:v>
+                  <c:v>738.08811644059426</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1298.7720040768052</c:v>
+                  <c:v>765.42471334580136</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1345.1567185081196</c:v>
+                  <c:v>792.76131025100858</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1391.5414329394341</c:v>
+                  <c:v>820.0979071562158</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1437.9261473707486</c:v>
+                  <c:v>847.43450406142301</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1484.3108618020633</c:v>
+                  <c:v>874.77110096663023</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1530.6955762333776</c:v>
+                  <c:v>902.10769787183733</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1577.080290664692</c:v>
+                  <c:v>929.44429477704455</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1623.4650050960065</c:v>
+                  <c:v>956.78089168225176</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6345,29 +6372,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A071DE-853C-4645-838D-52D3EBDAE5F1}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" customWidth="1"/>
-    <col min="7" max="11" width="14.53125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="10.265625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="7" max="11" width="14.5546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -6387,10 +6414,10 @@
         <v>32</v>
       </c>
       <c r="H5" s="16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
         <f>B5*12+D5</f>
         <v>98.25</v>
@@ -6399,7 +6426,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G7" s="5" t="s">
         <v>30</v>
       </c>
@@ -6416,7 +6443,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -6450,32 +6477,32 @@
         <v>74.25</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G9" s="3">
         <v>0.1</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="0"/>
-        <v>46.384714431314478</v>
+        <v>27.336596905207195</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" ref="I9:I43" si="2">H9/12</f>
-        <v>3.8653928692762065</v>
+        <v>2.2780497421005994</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>6.2471019465717816</v>
+        <v>25.398297539033234</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" ref="K9:K43" si="3">J9/12</f>
-        <v>0.52059182888098177</v>
+        <v>2.1165247949194361</v>
       </c>
       <c r="L9" s="3">
         <f t="shared" ref="L9:L43" si="4">$B$10</f>
         <v>74.25</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
@@ -6491,51 +6518,51 @@
       </c>
       <c r="H10" s="7">
         <f t="shared" si="0"/>
-        <v>92.769428862628956</v>
+        <v>54.673193810414389</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="2"/>
-        <v>7.730785738552413</v>
+        <v>4.5560994842011988</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="1"/>
-        <v>8.633803893143563</v>
+        <v>46.936195078066461</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="3"/>
-        <v>0.71948365776196355</v>
+        <v>3.9113495898388719</v>
       </c>
       <c r="L10" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G11" s="3">
         <v>0.3</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" si="0"/>
-        <v>139.15414329394341</v>
+        <v>82.009790715621577</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="2"/>
-        <v>11.596178607828618</v>
+        <v>6.8341492263017978</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" si="1"/>
-        <v>7.1601058397153459</v>
+        <v>64.613692617099701</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="3"/>
-        <v>0.59667548664294545</v>
+        <v>5.3844743847583088</v>
       </c>
       <c r="L11" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -6550,57 +6577,64 @@
       </c>
       <c r="H12" s="7">
         <f t="shared" si="0"/>
-        <v>185.53885772525791</v>
+        <v>109.34638762082878</v>
       </c>
       <c r="I12" s="7">
         <f t="shared" si="2"/>
-        <v>15.461571477104826</v>
+        <v>9.1121989684023976</v>
       </c>
       <c r="J12" s="7">
         <f t="shared" si="1"/>
-        <v>1.8260077862871213</v>
+        <v>78.430790156132929</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="3"/>
-        <v>0.15216731552392679</v>
+        <v>6.5358991796777444</v>
       </c>
       <c r="L12" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="12">
-        <v>6000</v>
+        <f>C13*D13</f>
+        <v>5423</v>
+      </c>
+      <c r="C13">
+        <v>0.85</v>
+      </c>
+      <c r="D13">
+        <v>6380</v>
       </c>
       <c r="G13" s="3">
         <v>0.5</v>
       </c>
       <c r="H13" s="7">
         <f t="shared" si="0"/>
-        <v>231.92357215657236</v>
+        <v>136.68298452603597</v>
       </c>
       <c r="I13" s="7">
         <f t="shared" si="2"/>
-        <v>19.326964346381029</v>
+        <v>11.390248710502997</v>
       </c>
       <c r="J13" s="7">
         <f t="shared" si="1"/>
-        <v>-7.368490267141091</v>
+        <v>88.387487695166158</v>
       </c>
       <c r="K13" s="7">
         <f t="shared" si="3"/>
-        <v>-0.61404085559509092</v>
+        <v>7.3656239745971801</v>
       </c>
       <c r="L13" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>22</v>
       </c>
@@ -6616,88 +6650,88 @@
       </c>
       <c r="H14" s="7">
         <f t="shared" si="0"/>
-        <v>278.30828658788681</v>
+        <v>164.01958143124315</v>
       </c>
       <c r="I14" s="7">
         <f t="shared" si="2"/>
-        <v>23.192357215657236</v>
+        <v>13.668298452603596</v>
       </c>
       <c r="J14" s="7">
         <f t="shared" si="1"/>
-        <v>-20.423388320569309</v>
+        <v>94.483785234199388</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="3"/>
-        <v>-1.7019490267141091</v>
+        <v>7.873648769516616</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="12">
-        <v>0.25</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="G15" s="3">
         <v>0.7</v>
       </c>
       <c r="H15" s="7">
         <f t="shared" si="0"/>
-        <v>324.69300101920129</v>
+        <v>191.35617833645034</v>
       </c>
       <c r="I15" s="7">
         <f t="shared" si="2"/>
-        <v>27.057750084933442</v>
+        <v>15.946348194704195</v>
       </c>
       <c r="J15" s="7">
         <f t="shared" si="1"/>
-        <v>-37.338686373997518</v>
+        <v>96.719682773232606</v>
       </c>
       <c r="K15" s="7">
         <f t="shared" si="3"/>
-        <v>-3.1115571978331267</v>
+        <v>8.0599735644360511</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G16" s="3">
         <v>0.8</v>
       </c>
       <c r="H16" s="7">
         <f t="shared" si="0"/>
-        <v>371.07771545051583</v>
+        <v>218.69277524165756</v>
       </c>
       <c r="I16" s="7">
         <f t="shared" si="2"/>
-        <v>30.923142954209652</v>
+        <v>18.224397936804795</v>
       </c>
       <c r="J16" s="7">
         <f t="shared" si="1"/>
-        <v>-58.114384427425776</v>
+        <v>95.095180312265825</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="3"/>
-        <v>-4.8428653689521477</v>
+        <v>7.9245983593554854</v>
       </c>
       <c r="L16" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="13">
         <f>B13*B14</f>
-        <v>113040</v>
+        <v>102169.31999999999</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
@@ -6707,32 +6741,32 @@
       </c>
       <c r="H17" s="7">
         <f t="shared" si="0"/>
-        <v>417.46242988183025</v>
+        <v>246.02937214686474</v>
       </c>
       <c r="I17" s="7">
         <f t="shared" si="2"/>
-        <v>34.788535823485851</v>
+        <v>20.502447678905394</v>
       </c>
       <c r="J17" s="7">
         <f t="shared" si="1"/>
-        <v>-82.750482480853961</v>
+        <v>89.61027785129906</v>
       </c>
       <c r="K17" s="7">
         <f t="shared" si="3"/>
-        <v>-6.8958735400711637</v>
+        <v>7.4675231542749216</v>
       </c>
       <c r="L17" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="15">
         <f>($B$15*B17)/(12*60)</f>
-        <v>39.25</v>
+        <v>32.211716166666669</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
@@ -6742,76 +6776,76 @@
       </c>
       <c r="H18" s="7">
         <f t="shared" si="0"/>
-        <v>463.84714431314472</v>
+        <v>273.36596905207193</v>
       </c>
       <c r="I18" s="7">
         <f t="shared" si="2"/>
-        <v>38.653928692762058</v>
+        <v>22.780497421005993</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" si="1"/>
-        <v>-111.24698053428219</v>
+        <v>80.264975390332296</v>
       </c>
       <c r="K18" s="7">
         <f t="shared" si="3"/>
-        <v>-9.2705817111901823</v>
+        <v>6.688747949194358</v>
       </c>
       <c r="L18" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G19" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="H19" s="7">
         <f t="shared" si="0"/>
-        <v>510.23185874445926</v>
+        <v>300.70256595727915</v>
       </c>
       <c r="I19" s="7">
         <f t="shared" si="2"/>
-        <v>42.519321562038272</v>
+        <v>25.058547163106596</v>
       </c>
       <c r="J19" s="7">
         <f t="shared" si="1"/>
-        <v>-143.60387858771043</v>
+        <v>67.059272929365534</v>
       </c>
       <c r="K19" s="7">
         <f t="shared" si="3"/>
-        <v>-11.966989882309202</v>
+        <v>5.5882727441137945</v>
       </c>
       <c r="L19" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G20" s="3">
         <v>1.2</v>
       </c>
       <c r="H20" s="7">
         <f t="shared" si="0"/>
-        <v>556.61657317577362</v>
+        <v>328.03916286248631</v>
       </c>
       <c r="I20" s="7">
         <f t="shared" si="2"/>
-        <v>46.384714431314471</v>
+        <v>27.336596905207191</v>
       </c>
       <c r="J20" s="7">
         <f t="shared" si="1"/>
-        <v>-179.82117664113861</v>
+        <v>49.993170468398773</v>
       </c>
       <c r="K20" s="7">
         <f t="shared" si="3"/>
-        <v>-14.985098053428217</v>
+        <v>4.1660975390332311</v>
       </c>
       <c r="L20" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -6826,26 +6860,26 @@
       </c>
       <c r="H21" s="7">
         <f t="shared" si="0"/>
-        <v>603.00128760708822</v>
+        <v>355.37575976769352</v>
       </c>
       <c r="I21" s="7">
         <f t="shared" si="2"/>
-        <v>50.250107300590685</v>
+        <v>29.614646647307794</v>
       </c>
       <c r="J21" s="7">
         <f t="shared" si="1"/>
-        <v>-219.89887469456687</v>
+        <v>29.066668007431929</v>
       </c>
       <c r="K21" s="7">
         <f t="shared" si="3"/>
-        <v>-18.324906224547238</v>
+        <v>2.4222223339526607</v>
       </c>
       <c r="L21" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B22">
         <f>B21*12</f>
         <v>386.04</v>
@@ -6858,151 +6892,151 @@
       </c>
       <c r="H22" s="7">
         <f t="shared" si="0"/>
-        <v>649.38600203840258</v>
+        <v>382.71235667290068</v>
       </c>
       <c r="I22" s="7">
         <f t="shared" si="2"/>
-        <v>54.115500169866884</v>
+        <v>31.892696389408389</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="1"/>
-        <v>-263.83697274799499</v>
+        <v>4.279765546465228</v>
       </c>
       <c r="K22" s="7">
         <f t="shared" si="3"/>
-        <v>-21.986414395666248</v>
+        <v>0.35664712887210231</v>
       </c>
       <c r="L22" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G23" s="3">
         <v>1.5</v>
       </c>
       <c r="H23" s="7">
         <f t="shared" si="0"/>
-        <v>695.77071646971706</v>
+        <v>410.0489535781079</v>
       </c>
       <c r="I23" s="7">
         <f t="shared" si="2"/>
-        <v>57.980893039143091</v>
+        <v>34.170746131508992</v>
       </c>
       <c r="J23" s="7">
         <f t="shared" si="1"/>
-        <v>-311.63547080142325</v>
+        <v>-24.367536914501557</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" si="3"/>
-        <v>-25.969622566785272</v>
+        <v>-2.0306280762084632</v>
       </c>
       <c r="L23" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G24" s="3">
         <v>1.6</v>
       </c>
       <c r="H24" s="7">
         <f t="shared" si="0"/>
-        <v>742.15543090103165</v>
+        <v>437.38555048331511</v>
       </c>
       <c r="I24" s="7">
         <f t="shared" si="2"/>
-        <v>61.846285908419304</v>
+        <v>36.448795873609591</v>
       </c>
       <c r="J24" s="7">
         <f t="shared" si="1"/>
-        <v>-363.29436885485165</v>
+        <v>-56.875239375468425</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" si="3"/>
-        <v>-30.274530737904303</v>
+        <v>-4.7396032812890354</v>
       </c>
       <c r="L24" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G25" s="3">
         <v>1.7</v>
       </c>
       <c r="H25" s="7">
         <f t="shared" si="0"/>
-        <v>788.54014533234601</v>
+        <v>464.72214738852227</v>
       </c>
       <c r="I25" s="7">
         <f t="shared" si="2"/>
-        <v>65.711678777695496</v>
+        <v>38.726845615710189</v>
       </c>
       <c r="J25" s="7">
         <f t="shared" si="1"/>
-        <v>-418.81366690827963</v>
+        <v>-93.243341836434979</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="3"/>
-        <v>-34.901138909023302</v>
+        <v>-7.7702784863695813</v>
       </c>
       <c r="L25" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G26" s="3">
         <v>1.8</v>
       </c>
       <c r="H26" s="7">
         <f t="shared" si="0"/>
-        <v>834.92485976366049</v>
+        <v>492.05874429372949</v>
       </c>
       <c r="I26" s="7">
         <f t="shared" si="2"/>
-        <v>69.577071646971703</v>
+        <v>41.004895357810788</v>
       </c>
       <c r="J26" s="7">
         <f t="shared" si="1"/>
-        <v>-478.19336496170797</v>
+        <v>-133.4718442974019</v>
       </c>
       <c r="K26" s="7">
         <f t="shared" si="3"/>
-        <v>-39.849447080142333</v>
+        <v>-11.122653691450159</v>
       </c>
       <c r="L26" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G27" s="3">
         <v>1.9</v>
       </c>
       <c r="H27" s="7">
         <f t="shared" si="0"/>
-        <v>881.30957419497497</v>
+        <v>519.39534119893665</v>
       </c>
       <c r="I27" s="7">
         <f t="shared" si="2"/>
-        <v>73.44246451624791</v>
+        <v>43.282945099911387</v>
       </c>
       <c r="J27" s="7">
         <f t="shared" si="1"/>
-        <v>-541.43346301513611</v>
+        <v>-177.56074675836862</v>
       </c>
       <c r="K27" s="7">
         <f t="shared" si="3"/>
-        <v>-45.119455251261343</v>
+        <v>-14.796728896530718</v>
       </c>
       <c r="L27" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="28" t="s">
         <v>35</v>
       </c>
@@ -7013,26 +7047,26 @@
       </c>
       <c r="H28" s="7">
         <f t="shared" si="0"/>
-        <v>927.69428862628945</v>
+        <v>546.73193810414386</v>
       </c>
       <c r="I28" s="7">
         <f t="shared" si="2"/>
-        <v>77.307857385524116</v>
+        <v>45.560994842011986</v>
       </c>
       <c r="J28" s="7">
         <f t="shared" si="1"/>
-        <v>-608.53396106856439</v>
+        <v>-225.51004921933543</v>
       </c>
       <c r="K28" s="7">
         <f t="shared" si="3"/>
-        <v>-50.711163422380366</v>
+        <v>-18.792504101611286</v>
       </c>
       <c r="L28" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
@@ -7041,26 +7075,26 @@
       </c>
       <c r="H29" s="7">
         <f t="shared" si="0"/>
-        <v>974.07900305760393</v>
+        <v>574.06853500935108</v>
       </c>
       <c r="I29" s="7">
         <f t="shared" si="2"/>
-        <v>81.173250254800323</v>
+        <v>47.839044584112592</v>
       </c>
       <c r="J29" s="7">
         <f t="shared" si="1"/>
-        <v>-679.49485912199259</v>
+        <v>-277.31975168030215</v>
       </c>
       <c r="K29" s="7">
         <f t="shared" si="3"/>
-        <v>-56.624571593499383</v>
+        <v>-23.109979306691844</v>
       </c>
       <c r="L29" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
         <v>36</v>
       </c>
@@ -7075,26 +7109,26 @@
       </c>
       <c r="H30" s="7">
         <f t="shared" si="0"/>
-        <v>1020.4637174889185</v>
+        <v>601.4051319145583</v>
       </c>
       <c r="I30" s="7">
         <f t="shared" si="2"/>
-        <v>85.038643124076543</v>
+        <v>50.117094326213191</v>
       </c>
       <c r="J30" s="7">
         <f t="shared" si="1"/>
-        <v>-754.31615717542093</v>
+        <v>-332.98985414126901</v>
       </c>
       <c r="K30" s="7">
         <f t="shared" si="3"/>
-        <v>-62.859679764618413</v>
+        <v>-27.749154511772417</v>
       </c>
       <c r="L30" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
@@ -7103,26 +7137,26 @@
       </c>
       <c r="H31" s="7">
         <f t="shared" si="0"/>
-        <v>1066.8484319202328</v>
+        <v>628.7417288197654</v>
       </c>
       <c r="I31" s="7">
         <f t="shared" si="2"/>
-        <v>88.904035993352736</v>
+        <v>52.395144068313783</v>
       </c>
       <c r="J31" s="7">
         <f t="shared" si="1"/>
-        <v>-832.99785522884883</v>
+        <v>-392.52035660223555</v>
       </c>
       <c r="K31" s="7">
         <f t="shared" si="3"/>
-        <v>-69.416487935737408</v>
+        <v>-32.710029716852965</v>
       </c>
       <c r="L31" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
         <v>32</v>
       </c>
@@ -7138,26 +7172,26 @@
       </c>
       <c r="H32" s="7">
         <f t="shared" si="0"/>
-        <v>1113.2331463515472</v>
+        <v>656.07832572497261</v>
       </c>
       <c r="I32" s="7">
         <f t="shared" si="2"/>
-        <v>92.769428862628942</v>
+        <v>54.673193810414382</v>
       </c>
       <c r="J32" s="7">
         <f t="shared" si="1"/>
-        <v>-915.53995328227722</v>
+        <v>-455.91125906320246</v>
       </c>
       <c r="K32" s="7">
         <f t="shared" si="3"/>
-        <v>-76.294996106856431</v>
+        <v>-37.992604921933541</v>
       </c>
       <c r="L32" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
@@ -7166,26 +7200,26 @@
       </c>
       <c r="H33" s="7">
         <f t="shared" si="0"/>
-        <v>1159.6178607828617</v>
+        <v>683.41492263017983</v>
       </c>
       <c r="I33" s="7">
         <f t="shared" si="2"/>
-        <v>96.634821731905149</v>
+        <v>56.951243552514988</v>
       </c>
       <c r="J33" s="7">
         <f t="shared" si="1"/>
-        <v>-1001.9424513357054</v>
+        <v>-523.16256152416918</v>
       </c>
       <c r="K33" s="7">
         <f t="shared" si="3"/>
-        <v>-83.495204277975446</v>
+        <v>-43.596880127014096</v>
       </c>
       <c r="L33" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
         <v>37</v>
       </c>
@@ -7201,26 +7235,26 @@
       </c>
       <c r="H34" s="7">
         <f t="shared" si="0"/>
-        <v>1206.0025752141764</v>
+        <v>710.75151953538705</v>
       </c>
       <c r="I34" s="7">
         <f t="shared" si="2"/>
-        <v>100.50021460118137</v>
+        <v>59.229293294615587</v>
       </c>
       <c r="J34" s="7">
         <f t="shared" si="1"/>
-        <v>-1092.205349389134</v>
+        <v>-594.27426398513626</v>
       </c>
       <c r="K34" s="7">
         <f t="shared" si="3"/>
-        <v>-91.017112449094498</v>
+        <v>-49.522855332094686</v>
       </c>
       <c r="L34" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
       <c r="B35" s="24">
         <f>ROUND(B34/12,1)</f>
@@ -7234,26 +7268,26 @@
       </c>
       <c r="H35" s="7">
         <f t="shared" si="0"/>
-        <v>1252.3872896454909</v>
+        <v>738.08811644059426</v>
       </c>
       <c r="I35" s="7">
         <f t="shared" si="2"/>
-        <v>104.36560747045758</v>
+        <v>61.507343036716186</v>
       </c>
       <c r="J35" s="7">
         <f t="shared" si="1"/>
-        <v>-1186.3286474425622</v>
+        <v>-669.24636644610302</v>
       </c>
       <c r="K35" s="7">
         <f t="shared" si="3"/>
-        <v>-98.860720620213513</v>
+        <v>-55.770530537175254</v>
       </c>
       <c r="L35" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="17"/>
       <c r="B36" s="18"/>
       <c r="C36" s="19"/>
@@ -7262,32 +7296,32 @@
       </c>
       <c r="H36" s="7">
         <f t="shared" si="0"/>
-        <v>1298.7720040768052</v>
+        <v>765.42471334580136</v>
       </c>
       <c r="I36" s="7">
         <f t="shared" si="2"/>
-        <v>108.23100033973377</v>
+        <v>63.785392778816778</v>
       </c>
       <c r="J36" s="7">
         <f t="shared" si="1"/>
-        <v>-1284.31234549599</v>
+        <v>-748.07886890706948</v>
       </c>
       <c r="K36" s="7">
         <f t="shared" si="3"/>
-        <v>-107.02602879133251</v>
+        <v>-62.339905742255787</v>
       </c>
       <c r="L36" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="21" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="25">
         <f>ROUND((720*B35)/(B15*B14),0)</f>
-        <v>9569</v>
+        <v>10539</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>41</v>
@@ -7297,234 +7331,234 @@
       </c>
       <c r="H37" s="7">
         <f t="shared" si="0"/>
-        <v>1345.1567185081196</v>
+        <v>792.76131025100858</v>
       </c>
       <c r="I37" s="7">
         <f t="shared" si="2"/>
-        <v>112.09639320900997</v>
+        <v>66.063442520917377</v>
       </c>
       <c r="J37" s="7">
         <f t="shared" si="1"/>
-        <v>-1386.1564435494186</v>
+        <v>-830.77177136803653</v>
       </c>
       <c r="K37" s="7">
         <f t="shared" si="3"/>
-        <v>-115.51303696245155</v>
+        <v>-69.230980947336377</v>
       </c>
       <c r="L37" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="G38" s="3">
         <v>3</v>
       </c>
       <c r="H38" s="7">
         <f t="shared" si="0"/>
-        <v>1391.5414329394341</v>
+        <v>820.0979071562158</v>
       </c>
       <c r="I38" s="7">
         <f t="shared" si="2"/>
-        <v>115.96178607828618</v>
+        <v>68.341492263017983</v>
       </c>
       <c r="J38" s="7">
         <f t="shared" si="1"/>
-        <v>-1491.8609416028467</v>
+        <v>-917.32507382900314</v>
       </c>
       <c r="K38" s="7">
         <f t="shared" si="3"/>
-        <v>-124.32174513357056</v>
+        <v>-76.443756152416924</v>
       </c>
       <c r="L38" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G39" s="3">
         <v>3.1</v>
       </c>
       <c r="H39" s="7">
         <f t="shared" si="0"/>
-        <v>1437.9261473707486</v>
+        <v>847.43450406142301</v>
       </c>
       <c r="I39" s="7">
         <f t="shared" si="2"/>
-        <v>119.82717894756239</v>
+        <v>70.619542005118589</v>
       </c>
       <c r="J39" s="7">
         <f t="shared" si="1"/>
-        <v>-1601.4258396562752</v>
+        <v>-1007.7387762899702</v>
       </c>
       <c r="K39" s="7">
         <f t="shared" si="3"/>
-        <v>-133.4521533046896</v>
+        <v>-83.978231357497521</v>
       </c>
       <c r="L39" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G40" s="3">
         <v>3.2</v>
       </c>
       <c r="H40" s="7">
         <f t="shared" si="0"/>
-        <v>1484.3108618020633</v>
+        <v>874.77110096663023</v>
       </c>
       <c r="I40" s="7">
         <f t="shared" si="2"/>
-        <v>123.69257181683861</v>
+        <v>72.897591747219181</v>
       </c>
       <c r="J40" s="7">
         <f t="shared" si="1"/>
-        <v>-1714.8511377097036</v>
+        <v>-1102.012878750937</v>
       </c>
       <c r="K40" s="7">
         <f t="shared" si="3"/>
-        <v>-142.90426147580862</v>
+        <v>-91.834406562578081</v>
       </c>
       <c r="L40" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G41" s="3">
         <v>3.3</v>
       </c>
       <c r="H41" s="7">
         <f t="shared" si="0"/>
-        <v>1530.6955762333776</v>
+        <v>902.10769787183733</v>
       </c>
       <c r="I41" s="7">
         <f t="shared" si="2"/>
-        <v>127.5579646861148</v>
+        <v>75.175641489319773</v>
       </c>
       <c r="J41" s="7">
         <f t="shared" si="1"/>
-        <v>-1832.1368357631311</v>
+        <v>-1200.1473812119034</v>
       </c>
       <c r="K41" s="7">
         <f t="shared" si="3"/>
-        <v>-152.67806964692758</v>
+        <v>-100.01228176765862</v>
       </c>
       <c r="L41" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G42" s="3">
         <v>3.4</v>
       </c>
       <c r="H42" s="7">
         <f t="shared" si="0"/>
-        <v>1577.080290664692</v>
+        <v>929.44429477704455</v>
       </c>
       <c r="I42" s="7">
         <f t="shared" si="2"/>
-        <v>131.42335755539099</v>
+        <v>77.453691231420379</v>
       </c>
       <c r="J42" s="7">
         <f t="shared" si="1"/>
-        <v>-1953.2829338165591</v>
+        <v>-1302.1422836728698</v>
       </c>
       <c r="K42" s="7">
         <f t="shared" si="3"/>
-        <v>-162.77357781804659</v>
+        <v>-108.51185697273915</v>
       </c>
       <c r="L42" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G43" s="3">
         <v>3.5</v>
       </c>
       <c r="H43" s="7">
         <f t="shared" si="0"/>
-        <v>1623.4650050960065</v>
+        <v>956.78089168225176</v>
       </c>
       <c r="I43" s="7">
         <f t="shared" si="2"/>
-        <v>135.2887504246672</v>
+        <v>79.731740973520985</v>
       </c>
       <c r="J43" s="7">
         <f t="shared" si="1"/>
-        <v>-2078.2894318699882</v>
+        <v>-1407.9975861338373</v>
       </c>
       <c r="K43" s="7">
         <f t="shared" si="3"/>
-        <v>-173.19078598916568</v>
+        <v>-117.33313217781978</v>
       </c>
       <c r="L43" s="3">
         <f t="shared" si="4"/>
         <v>74.25</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G48"/>
       <c r="H48"/>
       <c r="I48"/>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G49"/>
       <c r="H49"/>
     </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G50"/>
       <c r="H50"/>
     </row>
-    <row r="51" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G51"/>
       <c r="H51"/>
     </row>
-    <row r="52" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G52"/>
       <c r="H52"/>
     </row>
-    <row r="53" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G53"/>
       <c r="H53"/>
     </row>
-    <row r="54" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G54"/>
       <c r="H54"/>
     </row>
-    <row r="55" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G55"/>
       <c r="H55"/>
     </row>
-    <row r="56" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G56"/>
       <c r="H56"/>
     </row>
-    <row r="57" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G57"/>
       <c r="H57"/>
     </row>
-    <row r="58" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G58"/>
       <c r="H58"/>
     </row>
-    <row r="59" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G59"/>
       <c r="H59"/>
     </row>
-    <row r="60" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G60"/>
       <c r="H60"/>
     </row>
-    <row r="61" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G61"/>
       <c r="H61"/>
     </row>
@@ -7539,6 +7573,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB72D1B9-AB1F-4E81-B4BB-AF8902B9204F}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>0.95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>0.83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>0.9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>0.92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>0.91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60D84D8-D7E0-465A-92B3-61F1DC1412F6}">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -7546,17 +7666,17 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.53125" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -7564,7 +7684,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -7578,7 +7698,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>54</v>
       </c>
@@ -7599,7 +7719,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H7" t="s">
         <v>44</v>
       </c>
@@ -7611,7 +7731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I8" s="10">
         <f>ROUND(I7/12,1)</f>
         <v>18.399999999999999</v>
@@ -7620,17 +7740,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H10" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
@@ -7651,7 +7771,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>50</v>
       </c>
@@ -7672,7 +7792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -7690,7 +7810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>57</v>
       </c>
@@ -7701,7 +7821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
@@ -7717,7 +7837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A7A684-C6B9-48D0-BA62-41E5059F4BE2}">
   <dimension ref="A1:P75"/>
   <sheetViews>
@@ -7725,27 +7845,27 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" customWidth="1"/>
-    <col min="2" max="2" width="11.9296875" customWidth="1"/>
-    <col min="3" max="3" width="12.9296875" customWidth="1"/>
-    <col min="8" max="12" width="14.53125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="8" max="12" width="14.5546875" style="3" customWidth="1"/>
     <col min="13" max="13" width="17.6640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="14.53125" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -7780,7 +7900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>2.25</v>
       </c>
@@ -7795,7 +7915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H6" s="4" t="s">
         <v>6</v>
       </c>
@@ -7818,7 +7938,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -7857,7 +7977,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H8" s="3">
         <v>5</v>
       </c>
@@ -7889,7 +8009,7 @@
         <v>74.25</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -7930,7 +8050,7 @@
         <v>74.25</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C10">
         <f>C9*100</f>
         <v>981</v>
@@ -7969,7 +8089,7 @@
         <v>74.25</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H11" s="3">
         <v>5</v>
       </c>
@@ -8001,7 +8121,7 @@
         <v>74.25</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H12" s="3">
         <v>5</v>
       </c>
@@ -8033,7 +8153,7 @@
         <v>74.25</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H13" s="3">
         <v>5</v>
       </c>
@@ -8065,7 +8185,7 @@
         <v>74.25</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H14" s="3">
         <v>5</v>
       </c>
@@ -8097,7 +8217,7 @@
         <v>74.25</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H15" s="3">
         <v>5</v>
       </c>
@@ -8129,12 +8249,12 @@
         <v>74.25</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H18" s="4" t="s">
         <v>6</v>
       </c>
@@ -8157,7 +8277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -8189,7 +8309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>47</v>
       </c>
@@ -8226,7 +8346,7 @@
         <v>0.53123791386159191</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H21" s="3">
         <v>10</v>
       </c>
@@ -8254,7 +8374,7 @@
         <v>0.99842462216381322</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>6</v>
       </c>
@@ -8291,7 +8411,7 @@
         <v>1.3452315551505016</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -8328,7 +8448,7 @@
         <v>1.5298442986495295</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -8367,7 +8487,7 @@
         <v>1.530004146205288</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>25</v>
       </c>
@@ -8406,7 +8526,7 @@
         <v>1.3456918250430283</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>30</v>
       </c>
@@ -8445,7 +8565,7 @@
         <v>0.99912981978188053</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>35</v>
       </c>
@@ -8484,7 +8604,7 @@
         <v>0.53210301372713031</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>40</v>
       </c>
@@ -8497,7 +8617,7 @@
         <v>2.4338144731167453</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>45</v>
       </c>
@@ -8510,7 +8630,7 @@
         <v>2.0422717568628941</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>50</v>
       </c>
@@ -8544,7 +8664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>55</v>
       </c>
@@ -8578,7 +8698,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>60</v>
       </c>
@@ -8617,7 +8737,7 @@
         <v>2.1249516554463677</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>65</v>
       </c>
@@ -8656,7 +8776,7 @@
         <v>3.9936984886552529</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>70</v>
       </c>
@@ -8695,7 +8815,7 @@
         <v>5.3809262206020065</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>75</v>
       </c>
@@ -8734,7 +8854,7 @@
         <v>6.1193771945981181</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>80</v>
       </c>
@@ -8773,7 +8893,7 @@
         <v>6.1200165848211521</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="H37" s="3">
@@ -8803,7 +8923,7 @@
         <v>5.3827673001721132</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="H38" s="3">
@@ -8833,7 +8953,7 @@
         <v>3.9965192791275221</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="H39" s="3">
@@ -8863,15 +8983,15 @@
         <v>2.1284120549085213</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="H42" s="4" t="s">
@@ -8896,7 +9016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="H43" s="5" t="s">
@@ -8921,7 +9041,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="H44" s="3">
@@ -8951,7 +9071,7 @@
         <v>4.7811412247543261</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="H45" s="3">
@@ -8981,7 +9101,7 @@
         <v>8.9858215994743187</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="H46" s="3">
@@ -9011,7 +9131,7 @@
         <v>12.107083996354513</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="H47" s="3">
@@ -9041,7 +9161,7 @@
         <v>13.768598687845767</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="H48" s="3">
@@ -9071,7 +9191,7 @@
         <v>13.770037315847594</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="H49" s="3">
@@ -9101,7 +9221,7 @@
         <v>12.111226425387253</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H50" s="3">
         <v>30</v>
       </c>
@@ -9129,7 +9249,7 @@
         <v>8.9921683780369257</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H51" s="3">
         <v>30</v>
       </c>
@@ -9157,7 +9277,7 @@
         <v>4.7889271235441724</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H54" s="4" t="s">
         <v>6</v>
       </c>
@@ -9180,7 +9300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H55" s="5" t="s">
         <v>17</v>
       </c>
@@ -9203,7 +9323,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H56" s="3">
         <v>40</v>
       </c>
@@ -9231,7 +9351,7 @@
         <v>8.4998066217854706</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H57" s="3">
         <v>40</v>
       </c>
@@ -9259,7 +9379,7 @@
         <v>15.974793954621012</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H58" s="3">
         <v>40</v>
       </c>
@@ -9287,7 +9407,7 @@
         <v>21.523704882408026</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H59" s="3">
         <v>40</v>
       </c>
@@ -9315,7 +9435,7 @@
         <v>24.477508778392473</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H60" s="3">
         <v>40</v>
       </c>
@@ -9343,7 +9463,7 @@
         <v>24.480066339284608</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H61" s="3">
         <v>40</v>
       </c>
@@ -9371,7 +9491,7 @@
         <v>21.531069200688453</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H62" s="3">
         <v>40</v>
       </c>
@@ -9399,7 +9519,7 @@
         <v>15.986077116510089</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H63" s="3">
         <v>40</v>
       </c>
@@ -9427,7 +9547,7 @@
         <v>8.513648219634085</v>
       </c>
     </row>
-    <row r="66" spans="8:14" x14ac:dyDescent="0.45">
+    <row r="66" spans="8:14" x14ac:dyDescent="0.3">
       <c r="H66" s="4" t="s">
         <v>6</v>
       </c>
@@ -9450,7 +9570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="8:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="8:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H67" s="5" t="s">
         <v>17</v>
       </c>
@@ -9473,7 +9593,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="8:14" x14ac:dyDescent="0.45">
+    <row r="68" spans="8:14" x14ac:dyDescent="0.3">
       <c r="H68" s="3">
         <v>50</v>
       </c>
@@ -9501,7 +9621,7 @@
         <v>13.280947846539796</v>
       </c>
     </row>
-    <row r="69" spans="8:14" x14ac:dyDescent="0.45">
+    <row r="69" spans="8:14" x14ac:dyDescent="0.3">
       <c r="H69" s="3">
         <v>50</v>
       </c>
@@ -9529,7 +9649,7 @@
         <v>24.96061555409533</v>
       </c>
     </row>
-    <row r="70" spans="8:14" x14ac:dyDescent="0.45">
+    <row r="70" spans="8:14" x14ac:dyDescent="0.3">
       <c r="H70" s="3">
         <v>50</v>
       </c>
@@ -9557,7 +9677,7 @@
         <v>33.630788878762537</v>
       </c>
     </row>
-    <row r="71" spans="8:14" x14ac:dyDescent="0.45">
+    <row r="71" spans="8:14" x14ac:dyDescent="0.3">
       <c r="H71" s="3">
         <v>50</v>
       </c>
@@ -9585,7 +9705,7 @@
         <v>38.246107466238236</v>
       </c>
     </row>
-    <row r="72" spans="8:14" x14ac:dyDescent="0.45">
+    <row r="72" spans="8:14" x14ac:dyDescent="0.3">
       <c r="H72" s="3">
         <v>50</v>
       </c>
@@ -9613,7 +9733,7 @@
         <v>38.2501036551322</v>
       </c>
     </row>
-    <row r="73" spans="8:14" x14ac:dyDescent="0.45">
+    <row r="73" spans="8:14" x14ac:dyDescent="0.3">
       <c r="H73" s="3">
         <v>50</v>
       </c>
@@ -9641,7 +9761,7 @@
         <v>33.6422956260757</v>
       </c>
     </row>
-    <row r="74" spans="8:14" x14ac:dyDescent="0.45">
+    <row r="74" spans="8:14" x14ac:dyDescent="0.3">
       <c r="H74" s="3">
         <v>50</v>
       </c>
@@ -9669,7 +9789,7 @@
         <v>24.978245494547014</v>
       </c>
     </row>
-    <row r="75" spans="8:14" x14ac:dyDescent="0.45">
+    <row r="75" spans="8:14" x14ac:dyDescent="0.3">
       <c r="H75" s="3">
         <v>50</v>
       </c>
@@ -9703,7 +9823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9760CE-2D6D-4E8B-AFF0-30C50443C3C8}">
   <dimension ref="A2:F7"/>
   <sheetViews>
@@ -9711,14 +9831,14 @@
       <selection activeCell="B2" sqref="B2:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.796875" customWidth="1"/>
-    <col min="6" max="6" width="4.19921875" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" customWidth="1"/>
+    <col min="6" max="6" width="4.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
@@ -9739,7 +9859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>25</v>
       </c>
@@ -9750,7 +9870,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>26</v>
       </c>
@@ -9772,11 +9892,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>26</v>
       </c>
@@ -9792,7 +9912,7 @@
       </c>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>26</v>
       </c>

</xml_diff>